<commit_message>
see read datasets.py file to my my attempts at this.
</commit_message>
<xml_diff>
--- a/workspace/code/analyzer/file_processing/temporary_files/temp_format.xlsx
+++ b/workspace/code/analyzer/file_processing/temporary_files/temp_format.xlsx
@@ -1119,7 +1119,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31.25</t>
+          <t>29.00</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>10.65</t>
+          <t>10.25</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.45</t>
+          <t>2.30</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>21,492</t>
+          <t>20,919</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>8.10</t>
+          <t>8.00</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>444.65</t>
+          <t>326.95</t>
         </is>
       </c>
       <c r="N11" s="3" t="n"/>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>71.20</t>
+          <t>68.55</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>4.50</t>
+          <t>4.00</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1,587</t>
+          <t>1,747</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>950.20</t>
+          <t>1,013</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>10.30</t>
+          <t>10.20</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>30.35</t>
+          <t>31.50</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1,393</t>
+          <t>1,407</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>25.10</t>
+          <t>151.90</t>
         </is>
       </c>
     </row>

</xml_diff>